<commit_message>
Upload of most important problem
</commit_message>
<xml_diff>
--- a/Data/mip.xlsx
+++ b/Data/mip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lauriercloud-my.sharepoint.com/personal/skiss_wlu_ca/Documents/LISPOP/Surveys/Ontario_Housing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{191DB064-D98E-1F40-A94B-520D543049E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59976F12-A8DB-634E-99B3-6BADE1A580A3}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{191DB064-D98E-1F40-A94B-520D543049E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318AA716-2504-0E41-A130-F092324CEF78}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="500" windowWidth="18780" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15880" yWindow="1340" windowWidth="18780" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="965">
   <si>
     <t>mip</t>
   </si>
@@ -2920,6 +2920,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>mip_code</t>
   </si>
 </sst>
 </file>
@@ -3762,19 +3765,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C967"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C450" sqref="C450"/>
+    <sheetView tabSelected="1" topLeftCell="A680" workbookViewId="0">
+      <selection activeCell="B713" sqref="B713"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" customWidth="1"/>
+    <col min="1" max="1" width="123" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3805,7 +3811,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3981,7 +3987,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4028,8 +4034,8 @@
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>963</v>
+      <c r="B34">
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -4900,8 +4906,8 @@
       <c r="A143" t="s">
         <v>141</v>
       </c>
-      <c r="B143" t="s">
-        <v>963</v>
+      <c r="B143">
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -4972,8 +4978,8 @@
       <c r="A152" t="s">
         <v>150</v>
       </c>
-      <c r="B152" t="s">
-        <v>963</v>
+      <c r="B152">
+        <v>95</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -5004,8 +5010,8 @@
       <c r="A156" t="s">
         <v>154</v>
       </c>
-      <c r="B156" t="s">
-        <v>963</v>
+      <c r="B156">
+        <v>95</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -5781,8 +5787,8 @@
       <c r="A252" t="s">
         <v>250</v>
       </c>
-      <c r="B252" t="s">
-        <v>963</v>
+      <c r="B252">
+        <v>95</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
@@ -5968,8 +5974,8 @@
       <c r="A275" t="s">
         <v>272</v>
       </c>
-      <c r="B275" t="s">
-        <v>963</v>
+      <c r="B275">
+        <v>95</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -6147,8 +6153,8 @@
       <c r="A297" t="s">
         <v>294</v>
       </c>
-      <c r="B297" t="s">
-        <v>963</v>
+      <c r="B297">
+        <v>95</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
@@ -6886,8 +6892,8 @@
       <c r="A389" t="s">
         <v>386</v>
       </c>
-      <c r="B389" t="s">
-        <v>963</v>
+      <c r="B389">
+        <v>95</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
@@ -7014,8 +7020,8 @@
       <c r="A405" t="s">
         <v>402</v>
       </c>
-      <c r="B405" t="s">
-        <v>963</v>
+      <c r="B405">
+        <v>96</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
@@ -7070,8 +7076,8 @@
       <c r="A412" t="s">
         <v>409</v>
       </c>
-      <c r="B412" t="s">
-        <v>963</v>
+      <c r="B412">
+        <v>96</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
@@ -7342,16 +7348,16 @@
       <c r="A446" t="s">
         <v>443</v>
       </c>
-      <c r="B446" t="s">
-        <v>963</v>
+      <c r="B446">
+        <v>95</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>444</v>
       </c>
-      <c r="B447" t="s">
-        <v>963</v>
+      <c r="B447">
+        <v>95</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
@@ -7366,8 +7372,8 @@
       <c r="A449" t="s">
         <v>446</v>
       </c>
-      <c r="B449" t="s">
-        <v>963</v>
+      <c r="B449">
+        <v>96</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
@@ -7622,8 +7628,8 @@
       <c r="A481" t="s">
         <v>478</v>
       </c>
-      <c r="B481" t="s">
-        <v>963</v>
+      <c r="B481">
+        <v>96</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
@@ -7638,8 +7644,8 @@
       <c r="A483" t="s">
         <v>480</v>
       </c>
-      <c r="B483" t="s">
-        <v>963</v>
+      <c r="B483">
+        <v>97</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
@@ -8246,8 +8252,8 @@
       <c r="A559" t="s">
         <v>555</v>
       </c>
-      <c r="B559" t="s">
-        <v>963</v>
+      <c r="B559">
+        <v>95</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
@@ -8581,7 +8587,7 @@
         <v>595</v>
       </c>
       <c r="B600">
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.2">
@@ -8605,7 +8611,7 @@
         <v>598</v>
       </c>
       <c r="B603">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.2">
@@ -9032,7 +9038,7 @@
         <v>651</v>
       </c>
       <c r="B656">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
@@ -9371,7 +9377,7 @@
         <v>693</v>
       </c>
       <c r="B698">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C698" t="s">
         <v>963</v>
@@ -9486,7 +9492,7 @@
         <v>707</v>
       </c>
       <c r="B712">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C712">
         <v>12</v>

</xml_diff>